<commit_message>
Updated Command Give Donat Coins (givecoint [id] [amount])
Change currency from RedBucks to Coins
</commit_message>
<xml_diff>
--- a/Информация.xlsx
+++ b/Информация.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>ID</t>
   </si>
@@ -45,17 +45,44 @@
     <t>Заметки</t>
   </si>
   <si>
-    <t>[setproductbyindex]</t>
-  </si>
-  <si>
-    <t>[createbusiness]</t>
+    <t>givecoins</t>
+  </si>
+  <si>
+    <t>takecoins</t>
+  </si>
+  <si>
+    <t>[id] [количество]</t>
+  </si>
+  <si>
+    <t>[name] [количество]</t>
+  </si>
+  <si>
+    <t>Забрать донат валюту</t>
+  </si>
+  <si>
+    <t>Выдать донат валюту</t>
+  </si>
+  <si>
+    <t>Фикс</t>
+  </si>
+  <si>
+    <t>Да</t>
+  </si>
+  <si>
+    <t>Нет</t>
+  </si>
+  <si>
+    <t>createbusiness</t>
+  </si>
+  <si>
+    <t>setproductbyindex</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,8 +99,24 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -86,6 +129,16 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -96,10 +149,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -113,9 +168,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Плохой" xfId="2" builtinId="27"/>
+    <cellStyle name="Хороший" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -393,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -407,7 +497,7 @@
     <col min="4" max="4" width="30.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -420,78 +510,149 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="13">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="14">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="14"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="14">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="14"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="14">
+        <v>5</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="14"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="14">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="14"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="14">
+        <v>7</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="14"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="14">
+        <v>8</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="14"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
         <v>9</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+      <c r="B10" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="3"/>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="3"/>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="3"/>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="3"/>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="3"/>
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="3"/>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="3"/>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
-      <c r="C11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="15">
+        <v>10</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="3"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="3"/>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
       <c r="C16" s="2"/>
     </row>

</xml_diff>